<commit_message>
add material for final presentation
</commit_message>
<xml_diff>
--- a/evaluation/experiment_results/questionnaires/results_questionnaires.xlsx
+++ b/evaluation/experiment_results/questionnaires/results_questionnaires.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron-Spectre\gitRepos\coopsys-lego-ar-builder\evaluation\questionnaire\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron-Spectre\gitRepos\coopsys-lego-ar-builder\evaluation\experiment_results\questionnaires\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116C97D3-8A5F-46C2-8D29-4A92C00AAD8B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A7DF5A-F19C-4284-9113-267C8A889B30}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="840" windowWidth="29040" windowHeight="15480" activeTab="1" xr2:uid="{378B48E7-8773-405C-8223-FE28E6667752}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="22">
   <si>
     <t>ID</t>
   </si>
@@ -101,18 +101,6 @@
   <si>
     <t>Durchschnitt</t>
   </si>
-  <si>
-    <t>Summe</t>
-  </si>
-  <si>
-    <t>Mittelwert</t>
-  </si>
-  <si>
-    <t>Laufende Summe</t>
-  </si>
-  <si>
-    <t>Anzahl</t>
-  </si>
 </sst>
 </file>
 
@@ -120,7 +108,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -264,44 +252,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -314,15 +266,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -353,20 +296,65 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="2" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Ergebnis" xfId="2" builtinId="25"/>
@@ -639,7 +627,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -923,7 +910,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:schemeClr val="accent3"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1013,7 +1000,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent3"/>
+              <a:schemeClr val="accent5"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1103,7 +1090,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent4"/>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1456,7 +1445,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:schemeClr val="accent3"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1498,7 +1487,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent3"/>
+              <a:schemeClr val="accent5"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1540,7 +1529,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent4"/>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1820,13 +1811,10 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
   <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
   <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
   <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -1860,13 +1848,10 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
   <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
   <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
   <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -3833,172 +3818,172 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B733CBC6-756C-4ADB-90AE-44B4AD35AD46}">
   <dimension ref="A1:AE27"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AD37" sqref="AD37"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="19" width="11.42578125" style="41"/>
+    <col min="11" max="19" width="11.42578125" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="30"/>
-      <c r="C1" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="31" t="s">
+    <row r="1" spans="1:31" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="18"/>
+      <c r="C1" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="31" t="s">
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="42"/>
+      <c r="R1" s="42"/>
+      <c r="S1" s="42"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="33"/>
+      <c r="V1" s="42"/>
+      <c r="W1" s="42"/>
+      <c r="X1" s="42"/>
+      <c r="Y1" s="42"/>
+      <c r="Z1" s="42"/>
+      <c r="AA1" s="42"/>
+      <c r="AB1" s="42"/>
+      <c r="AC1" s="42"/>
+      <c r="AD1" s="42"/>
+      <c r="AE1" s="43"/>
     </row>
-    <row r="2" spans="1:31" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="25" t="s">
+    <row r="2" spans="1:31" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="26">
-        <v>2</v>
-      </c>
-      <c r="D2" s="24">
+      <c r="C2" s="14">
+        <v>2</v>
+      </c>
+      <c r="D2" s="12">
         <v>3</v>
       </c>
-      <c r="E2" s="24">
-        <v>4</v>
-      </c>
-      <c r="F2" s="24">
-        <v>5</v>
-      </c>
-      <c r="G2" s="24">
+      <c r="E2" s="12">
+        <v>4</v>
+      </c>
+      <c r="F2" s="12">
+        <v>5</v>
+      </c>
+      <c r="G2" s="12">
         <v>6</v>
       </c>
-      <c r="H2" s="24">
+      <c r="H2" s="12">
         <v>7</v>
       </c>
-      <c r="I2" s="27">
+      <c r="I2" s="15">
         <v>8</v>
       </c>
-      <c r="J2" s="26"/>
-      <c r="K2" s="37">
-        <v>1</v>
-      </c>
-      <c r="L2" s="37">
-        <v>2</v>
-      </c>
-      <c r="M2" s="37">
+      <c r="J2" s="14"/>
+      <c r="K2" s="22">
+        <v>1</v>
+      </c>
+      <c r="L2" s="22">
+        <v>2</v>
+      </c>
+      <c r="M2" s="22">
         <v>3</v>
       </c>
-      <c r="N2" s="37">
-        <v>4</v>
-      </c>
-      <c r="O2" s="37">
-        <v>5</v>
-      </c>
-      <c r="P2" s="37">
+      <c r="N2" s="22">
+        <v>4</v>
+      </c>
+      <c r="O2" s="22">
+        <v>5</v>
+      </c>
+      <c r="P2" s="22">
         <v>6</v>
       </c>
-      <c r="Q2" s="37">
+      <c r="Q2" s="22">
         <v>7</v>
       </c>
-      <c r="R2" s="37">
+      <c r="R2" s="22">
         <v>8</v>
       </c>
-      <c r="S2" s="37">
+      <c r="S2" s="22">
         <v>9</v>
       </c>
-      <c r="T2" s="28" t="s">
+      <c r="T2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="U2" s="24"/>
-      <c r="V2" s="24">
-        <v>1</v>
-      </c>
-      <c r="W2" s="24">
-        <v>2</v>
-      </c>
-      <c r="X2" s="24">
+      <c r="U2" s="12"/>
+      <c r="V2" s="12">
+        <v>1</v>
+      </c>
+      <c r="W2" s="12">
+        <v>2</v>
+      </c>
+      <c r="X2" s="12">
         <v>3</v>
       </c>
-      <c r="Y2" s="24">
-        <v>4</v>
-      </c>
-      <c r="Z2" s="24">
-        <v>5</v>
-      </c>
-      <c r="AA2" s="24">
+      <c r="Y2" s="12">
+        <v>4</v>
+      </c>
+      <c r="Z2" s="12">
+        <v>5</v>
+      </c>
+      <c r="AA2" s="12">
         <v>6</v>
       </c>
-      <c r="AB2" s="24">
+      <c r="AB2" s="12">
         <v>7</v>
       </c>
-      <c r="AC2" s="24">
+      <c r="AC2" s="12">
         <v>8</v>
       </c>
-      <c r="AD2" s="24">
+      <c r="AD2" s="12">
         <v>9</v>
       </c>
-      <c r="AE2" s="28" t="s">
+      <c r="AE2" s="16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:31" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="34"/>
-      <c r="C3" s="35"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="38"/>
-      <c r="P3" s="38"/>
-      <c r="Q3" s="38"/>
-      <c r="R3" s="38"/>
-      <c r="S3" s="38"/>
-      <c r="T3" s="36"/>
-      <c r="AE3" s="36"/>
+    <row r="3" spans="1:31" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="21"/>
+      <c r="AE3" s="21"/>
     </row>
     <row r="4" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="44" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="5">
         <v>1</v>
       </c>
-      <c r="C4" s="50">
+      <c r="C4" s="33">
         <v>23</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -4022,34 +4007,34 @@
       <c r="J4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="39">
+      <c r="K4" s="24">
         <v>3</v>
       </c>
-      <c r="L4" s="39">
-        <v>5</v>
-      </c>
-      <c r="M4" s="39">
-        <v>4</v>
-      </c>
-      <c r="N4" s="40">
-        <v>4</v>
-      </c>
-      <c r="O4" s="40">
-        <v>5</v>
-      </c>
-      <c r="P4" s="40">
-        <v>5</v>
-      </c>
-      <c r="Q4" s="40">
-        <v>5</v>
-      </c>
-      <c r="R4" s="40">
-        <v>5</v>
-      </c>
-      <c r="S4" s="39">
-        <v>4</v>
-      </c>
-      <c r="T4" s="46">
+      <c r="L4" s="24">
+        <v>5</v>
+      </c>
+      <c r="M4" s="24">
+        <v>4</v>
+      </c>
+      <c r="N4" s="25">
+        <v>4</v>
+      </c>
+      <c r="O4" s="25">
+        <v>5</v>
+      </c>
+      <c r="P4" s="25">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="25">
+        <v>5</v>
+      </c>
+      <c r="R4" s="25">
+        <v>5</v>
+      </c>
+      <c r="S4" s="24">
+        <v>4</v>
+      </c>
+      <c r="T4" s="40">
         <v>2.7083333333333334E-2</v>
       </c>
       <c r="U4" s="3" t="s">
@@ -4082,16 +4067,16 @@
       <c r="AD4" s="3">
         <v>1</v>
       </c>
-      <c r="AE4" s="46">
+      <c r="AE4" s="40">
         <v>2.7083333333333334E-2</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
+      <c r="A5" s="44"/>
       <c r="B5" s="5">
         <v>2</v>
       </c>
-      <c r="C5" s="50">
+      <c r="C5" s="33">
         <v>21</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -4115,34 +4100,34 @@
       <c r="J5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="39">
-        <v>5</v>
-      </c>
-      <c r="L5" s="39">
-        <v>4</v>
-      </c>
-      <c r="M5" s="40">
-        <v>5</v>
-      </c>
-      <c r="N5" s="40">
-        <v>4</v>
-      </c>
-      <c r="O5" s="40">
-        <v>4</v>
-      </c>
-      <c r="P5" s="40">
-        <v>5</v>
-      </c>
-      <c r="Q5" s="40">
+      <c r="K5" s="24">
+        <v>5</v>
+      </c>
+      <c r="L5" s="24">
+        <v>4</v>
+      </c>
+      <c r="M5" s="25">
+        <v>5</v>
+      </c>
+      <c r="N5" s="25">
+        <v>4</v>
+      </c>
+      <c r="O5" s="25">
+        <v>4</v>
+      </c>
+      <c r="P5" s="25">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="25">
         <v>3</v>
       </c>
-      <c r="R5" s="40">
-        <v>5</v>
-      </c>
-      <c r="S5" s="39">
-        <v>1</v>
-      </c>
-      <c r="T5" s="46"/>
+      <c r="R5" s="25">
+        <v>5</v>
+      </c>
+      <c r="S5" s="24">
+        <v>1</v>
+      </c>
+      <c r="T5" s="40"/>
       <c r="U5" s="3" t="s">
         <v>12</v>
       </c>
@@ -4173,12 +4158,12 @@
       <c r="AD5" s="3">
         <v>2</v>
       </c>
-      <c r="AE5" s="46"/>
+      <c r="AE5" s="40"/>
     </row>
     <row r="6" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="5"/>
-      <c r="C6" s="50"/>
+      <c r="C6" s="33"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -4186,16 +4171,16 @@
       <c r="H6" s="3"/>
       <c r="I6" s="5"/>
       <c r="J6" s="8"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="39"/>
-      <c r="M6" s="39"/>
-      <c r="N6" s="39"/>
-      <c r="O6" s="39"/>
-      <c r="P6" s="39"/>
-      <c r="Q6" s="39"/>
-      <c r="R6" s="39"/>
-      <c r="S6" s="39"/>
-      <c r="T6" s="47"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="24"/>
+      <c r="S6" s="24"/>
+      <c r="T6" s="31"/>
       <c r="U6" s="3"/>
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
@@ -4206,14 +4191,14 @@
       <c r="AB6" s="3"/>
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
-      <c r="AE6" s="47"/>
+      <c r="AE6" s="31"/>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="5">
         <v>3</v>
       </c>
-      <c r="C7" s="50">
+      <c r="C7" s="33">
         <v>24</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -4237,34 +4222,34 @@
       <c r="J7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="40">
-        <v>2</v>
-      </c>
-      <c r="L7" s="40">
-        <v>5</v>
-      </c>
-      <c r="M7" s="40">
-        <v>5</v>
-      </c>
-      <c r="N7" s="40">
+      <c r="K7" s="25">
+        <v>2</v>
+      </c>
+      <c r="L7" s="25">
+        <v>5</v>
+      </c>
+      <c r="M7" s="25">
+        <v>5</v>
+      </c>
+      <c r="N7" s="25">
         <v>3</v>
       </c>
-      <c r="O7" s="40">
+      <c r="O7" s="25">
         <v>3</v>
       </c>
-      <c r="P7" s="40">
-        <v>5</v>
-      </c>
-      <c r="Q7" s="40">
+      <c r="P7" s="25">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="25">
         <v>3</v>
       </c>
-      <c r="R7" s="40">
+      <c r="R7" s="25">
         <v>3</v>
       </c>
-      <c r="S7" s="39">
-        <v>1</v>
-      </c>
-      <c r="T7" s="46">
+      <c r="S7" s="24">
+        <v>1</v>
+      </c>
+      <c r="T7" s="40">
         <v>3.9583333333333331E-2</v>
       </c>
       <c r="U7" s="3" t="s">
@@ -4297,16 +4282,16 @@
       <c r="AD7" s="3">
         <v>1</v>
       </c>
-      <c r="AE7" s="46">
+      <c r="AE7" s="40">
         <v>2.2916666666666669E-2</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="5">
         <v>4</v>
       </c>
-      <c r="C8" s="51">
+      <c r="C8" s="34">
         <v>24</v>
       </c>
       <c r="D8" s="9" t="s">
@@ -4330,34 +4315,34 @@
       <c r="J8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K8" s="40">
+      <c r="K8" s="25">
         <v>3</v>
       </c>
-      <c r="L8" s="40">
-        <v>5</v>
-      </c>
-      <c r="M8" s="40">
-        <v>2</v>
-      </c>
-      <c r="N8" s="40">
+      <c r="L8" s="25">
+        <v>5</v>
+      </c>
+      <c r="M8" s="25">
+        <v>2</v>
+      </c>
+      <c r="N8" s="25">
         <v>3</v>
       </c>
-      <c r="O8" s="40">
-        <v>5</v>
-      </c>
-      <c r="P8" s="40">
-        <v>4</v>
-      </c>
-      <c r="Q8" s="40">
-        <v>2</v>
-      </c>
-      <c r="R8" s="40">
-        <v>4</v>
-      </c>
-      <c r="S8" s="39">
-        <v>2</v>
-      </c>
-      <c r="T8" s="46"/>
+      <c r="O8" s="25">
+        <v>5</v>
+      </c>
+      <c r="P8" s="25">
+        <v>4</v>
+      </c>
+      <c r="Q8" s="25">
+        <v>2</v>
+      </c>
+      <c r="R8" s="25">
+        <v>4</v>
+      </c>
+      <c r="S8" s="24">
+        <v>2</v>
+      </c>
+      <c r="T8" s="40"/>
       <c r="U8" s="9" t="s">
         <v>12</v>
       </c>
@@ -4388,12 +4373,12 @@
       <c r="AD8" s="3">
         <v>1</v>
       </c>
-      <c r="AE8" s="46"/>
+      <c r="AE8" s="40"/>
     </row>
     <row r="9" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="52"/>
+      <c r="C9" s="35"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -4401,16 +4386,16 @@
       <c r="H9" s="3"/>
       <c r="I9" s="5"/>
       <c r="J9" s="8"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="39"/>
-      <c r="N9" s="39"/>
-      <c r="O9" s="39"/>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="39"/>
-      <c r="R9" s="39"/>
-      <c r="S9" s="39"/>
-      <c r="T9" s="47"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="24"/>
+      <c r="T9" s="31"/>
       <c r="U9" s="3"/>
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
@@ -4421,14 +4406,14 @@
       <c r="AB9" s="3"/>
       <c r="AC9" s="3"/>
       <c r="AD9" s="3"/>
-      <c r="AE9" s="47"/>
+      <c r="AE9" s="31"/>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="5">
         <v>5</v>
       </c>
-      <c r="C10" s="53">
+      <c r="C10" s="36">
         <v>32</v>
       </c>
       <c r="D10" s="9" t="s">
@@ -4452,34 +4437,34 @@
       <c r="J10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="40">
+      <c r="K10" s="25">
         <v>3</v>
       </c>
-      <c r="L10" s="40">
-        <v>4</v>
-      </c>
-      <c r="M10" s="40">
-        <v>1</v>
-      </c>
-      <c r="N10" s="40">
+      <c r="L10" s="25">
+        <v>4</v>
+      </c>
+      <c r="M10" s="25">
+        <v>1</v>
+      </c>
+      <c r="N10" s="25">
         <v>3</v>
       </c>
-      <c r="O10" s="40">
-        <v>5</v>
-      </c>
-      <c r="P10" s="40">
-        <v>5</v>
-      </c>
-      <c r="Q10" s="40">
-        <v>5</v>
-      </c>
-      <c r="R10" s="40">
-        <v>5</v>
-      </c>
-      <c r="S10" s="40">
-        <v>4</v>
-      </c>
-      <c r="T10" s="46">
+      <c r="O10" s="25">
+        <v>5</v>
+      </c>
+      <c r="P10" s="25">
+        <v>5</v>
+      </c>
+      <c r="Q10" s="25">
+        <v>5</v>
+      </c>
+      <c r="R10" s="25">
+        <v>5</v>
+      </c>
+      <c r="S10" s="25">
+        <v>4</v>
+      </c>
+      <c r="T10" s="40">
         <v>4.3750000000000004E-2</v>
       </c>
       <c r="U10" s="9" t="s">
@@ -4512,16 +4497,16 @@
       <c r="AD10" s="9">
         <v>2</v>
       </c>
-      <c r="AE10" s="46">
+      <c r="AE10" s="40">
         <v>4.7916666666666663E-2</v>
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
+      <c r="A11" s="44"/>
       <c r="B11" s="5">
         <v>6</v>
       </c>
-      <c r="C11" s="52">
+      <c r="C11" s="35">
         <v>32</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -4545,34 +4530,34 @@
       <c r="J11" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="K11" s="39">
-        <v>5</v>
-      </c>
-      <c r="L11" s="39">
-        <v>5</v>
-      </c>
-      <c r="M11" s="39">
-        <v>4</v>
-      </c>
-      <c r="N11" s="39">
-        <v>2</v>
-      </c>
-      <c r="O11" s="39">
-        <v>5</v>
-      </c>
-      <c r="P11" s="39">
-        <v>5</v>
-      </c>
-      <c r="Q11" s="39">
-        <v>2</v>
-      </c>
-      <c r="R11" s="39">
-        <v>5</v>
-      </c>
-      <c r="S11" s="39">
-        <v>4</v>
-      </c>
-      <c r="T11" s="46"/>
+      <c r="K11" s="24">
+        <v>5</v>
+      </c>
+      <c r="L11" s="24">
+        <v>5</v>
+      </c>
+      <c r="M11" s="24">
+        <v>4</v>
+      </c>
+      <c r="N11" s="24">
+        <v>2</v>
+      </c>
+      <c r="O11" s="24">
+        <v>5</v>
+      </c>
+      <c r="P11" s="24">
+        <v>5</v>
+      </c>
+      <c r="Q11" s="24">
+        <v>2</v>
+      </c>
+      <c r="R11" s="24">
+        <v>5</v>
+      </c>
+      <c r="S11" s="24">
+        <v>4</v>
+      </c>
+      <c r="T11" s="40"/>
       <c r="U11" s="3" t="s">
         <v>9</v>
       </c>
@@ -4603,104 +4588,104 @@
       <c r="AD11" s="3">
         <v>2</v>
       </c>
-      <c r="AE11" s="46"/>
+      <c r="AE11" s="40"/>
     </row>
-    <row r="12" spans="1:31" s="43" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="42"/>
-      <c r="B12" s="43" t="s">
+    <row r="12" spans="1:31" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="27"/>
+      <c r="B12" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="45">
+      <c r="C12" s="30">
         <f>AVERAGE(C4:C11)</f>
         <v>26</v>
       </c>
-      <c r="H12" s="45">
+      <c r="H12" s="30">
         <f>AVERAGE(H5:H11)</f>
         <v>4.5999999999999996</v>
       </c>
-      <c r="K12" s="44">
+      <c r="K12" s="29">
         <f>AVERAGE(K4:K11)</f>
         <v>3.5</v>
       </c>
-      <c r="L12" s="44">
+      <c r="L12" s="29">
         <f t="shared" ref="L12:S12" si="0">AVERAGE(L4:L11)</f>
         <v>4.666666666666667</v>
       </c>
-      <c r="M12" s="44">
+      <c r="M12" s="29">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="N12" s="44">
+      <c r="N12" s="29">
         <f t="shared" si="0"/>
         <v>3.1666666666666665</v>
       </c>
-      <c r="O12" s="44">
+      <c r="O12" s="29">
         <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
-      <c r="P12" s="44">
+      <c r="P12" s="29">
         <f t="shared" si="0"/>
         <v>4.833333333333333</v>
       </c>
-      <c r="Q12" s="44">
+      <c r="Q12" s="29">
         <f t="shared" si="0"/>
         <v>3.3333333333333335</v>
       </c>
-      <c r="R12" s="44">
+      <c r="R12" s="29">
         <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
-      <c r="S12" s="44">
+      <c r="S12" s="29">
         <f t="shared" si="0"/>
         <v>2.6666666666666665</v>
       </c>
-      <c r="T12" s="48">
+      <c r="T12" s="32">
         <f>AVERAGE(T4:T11)</f>
         <v>3.6805555555555557E-2</v>
       </c>
-      <c r="V12" s="43">
+      <c r="V12" s="28">
         <f>AVERAGE(V4:V11)</f>
         <v>4.833333333333333</v>
       </c>
-      <c r="W12" s="43">
+      <c r="W12" s="28">
         <f t="shared" ref="W12:AD12" si="1">AVERAGE(W4:W11)</f>
         <v>4.5</v>
       </c>
-      <c r="X12" s="43">
+      <c r="X12" s="28">
         <f t="shared" si="1"/>
         <v>4.166666666666667</v>
       </c>
-      <c r="Y12" s="43">
+      <c r="Y12" s="28">
         <f t="shared" si="1"/>
         <v>4.166666666666667</v>
       </c>
-      <c r="Z12" s="43">
+      <c r="Z12" s="28">
         <f t="shared" si="1"/>
         <v>2.8333333333333335</v>
       </c>
-      <c r="AA12" s="43">
+      <c r="AA12" s="28">
         <f t="shared" si="1"/>
         <v>4.333333333333333</v>
       </c>
-      <c r="AB12" s="43">
+      <c r="AB12" s="28">
         <f t="shared" si="1"/>
         <v>1.6666666666666667</v>
       </c>
-      <c r="AC12" s="43">
+      <c r="AC12" s="28">
         <f t="shared" si="1"/>
         <v>4.666666666666667</v>
       </c>
-      <c r="AD12" s="43">
+      <c r="AD12" s="28">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
-      <c r="AE12" s="48">
+      <c r="AE12" s="32">
         <f>AVERAGE(AE4:AE11)</f>
         <v>3.2638888888888891E-2</v>
       </c>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="37" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="5">
@@ -4730,34 +4715,34 @@
       <c r="J13" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K13" s="40">
+      <c r="K13" s="25">
         <v>3</v>
       </c>
-      <c r="L13" s="40">
-        <v>4</v>
-      </c>
-      <c r="M13" s="40">
+      <c r="L13" s="25">
+        <v>4</v>
+      </c>
+      <c r="M13" s="25">
         <v>3</v>
       </c>
-      <c r="N13" s="40">
-        <v>2</v>
-      </c>
-      <c r="O13" s="40">
-        <v>2</v>
-      </c>
-      <c r="P13" s="40">
-        <v>4</v>
-      </c>
-      <c r="Q13" s="40">
-        <v>4</v>
-      </c>
-      <c r="R13" s="40">
-        <v>5</v>
-      </c>
-      <c r="S13" s="40">
-        <v>2</v>
-      </c>
-      <c r="T13" s="49">
+      <c r="N13" s="25">
+        <v>2</v>
+      </c>
+      <c r="O13" s="25">
+        <v>2</v>
+      </c>
+      <c r="P13" s="25">
+        <v>4</v>
+      </c>
+      <c r="Q13" s="25">
+        <v>4</v>
+      </c>
+      <c r="R13" s="25">
+        <v>5</v>
+      </c>
+      <c r="S13" s="25">
+        <v>2</v>
+      </c>
+      <c r="T13" s="39">
         <v>0.1111111111111111</v>
       </c>
       <c r="U13" s="8" t="s">
@@ -4790,12 +4775,12 @@
       <c r="AD13" s="9">
         <v>2</v>
       </c>
-      <c r="AE13" s="49">
+      <c r="AE13" s="39">
         <v>1.8749999999999999E-2</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
+      <c r="A14" s="38"/>
       <c r="B14" s="5">
         <v>8</v>
       </c>
@@ -4823,34 +4808,34 @@
       <c r="J14" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K14" s="40">
-        <v>5</v>
-      </c>
-      <c r="L14" s="40">
-        <v>5</v>
-      </c>
-      <c r="M14" s="40">
+      <c r="K14" s="25">
+        <v>5</v>
+      </c>
+      <c r="L14" s="25">
+        <v>5</v>
+      </c>
+      <c r="M14" s="25">
         <v>3</v>
       </c>
-      <c r="N14" s="40">
-        <v>4</v>
-      </c>
-      <c r="O14" s="40">
+      <c r="N14" s="25">
+        <v>4</v>
+      </c>
+      <c r="O14" s="25">
         <v>3</v>
       </c>
-      <c r="P14" s="40">
-        <v>4</v>
-      </c>
-      <c r="Q14" s="40">
-        <v>4</v>
-      </c>
-      <c r="R14" s="40">
-        <v>4</v>
-      </c>
-      <c r="S14" s="40">
-        <v>2</v>
-      </c>
-      <c r="T14" s="46"/>
+      <c r="P14" s="25">
+        <v>4</v>
+      </c>
+      <c r="Q14" s="25">
+        <v>4</v>
+      </c>
+      <c r="R14" s="25">
+        <v>4</v>
+      </c>
+      <c r="S14" s="25">
+        <v>2</v>
+      </c>
+      <c r="T14" s="40"/>
       <c r="U14" s="8" t="s">
         <v>12</v>
       </c>
@@ -4881,17 +4866,17 @@
       <c r="AD14" s="9">
         <v>2</v>
       </c>
-      <c r="AE14" s="46"/>
+      <c r="AE14" s="40"/>
     </row>
     <row r="15" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
+      <c r="A15" s="38"/>
       <c r="B15" s="5"/>
       <c r="I15" s="5"/>
-      <c r="T15" s="47"/>
-      <c r="AE15" s="47"/>
+      <c r="T15" s="31"/>
+      <c r="AE15" s="31"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
+      <c r="A16" s="38"/>
       <c r="B16" s="5">
         <v>9</v>
       </c>
@@ -4919,34 +4904,34 @@
       <c r="J16" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="K16" s="40">
-        <v>4</v>
-      </c>
-      <c r="L16" s="40">
-        <v>4</v>
-      </c>
-      <c r="M16" s="40">
-        <v>4</v>
-      </c>
-      <c r="N16" s="40">
-        <v>5</v>
-      </c>
-      <c r="O16" s="40">
-        <v>4</v>
-      </c>
-      <c r="P16" s="40">
-        <v>4</v>
-      </c>
-      <c r="Q16" s="40">
+      <c r="K16" s="25">
+        <v>4</v>
+      </c>
+      <c r="L16" s="25">
+        <v>4</v>
+      </c>
+      <c r="M16" s="25">
+        <v>4</v>
+      </c>
+      <c r="N16" s="25">
+        <v>5</v>
+      </c>
+      <c r="O16" s="25">
+        <v>4</v>
+      </c>
+      <c r="P16" s="25">
+        <v>4</v>
+      </c>
+      <c r="Q16" s="25">
         <v>3</v>
       </c>
-      <c r="R16" s="40">
-        <v>4</v>
-      </c>
-      <c r="S16" s="40">
-        <v>1</v>
-      </c>
-      <c r="T16" s="46">
+      <c r="R16" s="25">
+        <v>4</v>
+      </c>
+      <c r="S16" s="25">
+        <v>1</v>
+      </c>
+      <c r="T16" s="40">
         <v>6.0416666666666667E-2</v>
       </c>
       <c r="U16" s="10" t="s">
@@ -4979,12 +4964,12 @@
       <c r="AD16" s="9">
         <v>1</v>
       </c>
-      <c r="AE16" s="46">
+      <c r="AE16" s="40">
         <v>2.361111111111111E-2</v>
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
+      <c r="A17" s="38"/>
       <c r="B17" s="5">
         <v>10</v>
       </c>
@@ -5012,34 +4997,34 @@
       <c r="J17" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="K17" s="40">
-        <v>4</v>
-      </c>
-      <c r="L17" s="40">
+      <c r="K17" s="25">
+        <v>4</v>
+      </c>
+      <c r="L17" s="25">
         <v>3</v>
       </c>
-      <c r="M17" s="40">
-        <v>2</v>
-      </c>
-      <c r="N17" s="40">
-        <v>5</v>
-      </c>
-      <c r="O17" s="40">
-        <v>4</v>
-      </c>
-      <c r="P17" s="40">
-        <v>5</v>
-      </c>
-      <c r="Q17" s="40">
-        <v>4</v>
-      </c>
-      <c r="R17" s="40">
-        <v>4</v>
-      </c>
-      <c r="S17" s="40">
-        <v>1</v>
-      </c>
-      <c r="T17" s="46"/>
+      <c r="M17" s="25">
+        <v>2</v>
+      </c>
+      <c r="N17" s="25">
+        <v>5</v>
+      </c>
+      <c r="O17" s="25">
+        <v>4</v>
+      </c>
+      <c r="P17" s="25">
+        <v>5</v>
+      </c>
+      <c r="Q17" s="25">
+        <v>4</v>
+      </c>
+      <c r="R17" s="25">
+        <v>4</v>
+      </c>
+      <c r="S17" s="25">
+        <v>1</v>
+      </c>
+      <c r="T17" s="40"/>
       <c r="U17" s="8" t="s">
         <v>12</v>
       </c>
@@ -5070,10 +5055,10 @@
       <c r="AD17" s="9">
         <v>1</v>
       </c>
-      <c r="AE17" s="46"/>
+      <c r="AE17" s="40"/>
     </row>
     <row r="18" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
+      <c r="A18" s="38"/>
       <c r="B18" s="5"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -5083,16 +5068,16 @@
       <c r="H18" s="3"/>
       <c r="I18" s="5"/>
       <c r="J18" s="3"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="39"/>
-      <c r="M18" s="39"/>
-      <c r="N18" s="39"/>
-      <c r="O18" s="39"/>
-      <c r="P18" s="39"/>
-      <c r="Q18" s="39"/>
-      <c r="R18" s="39"/>
-      <c r="S18" s="39"/>
-      <c r="T18" s="47"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="24"/>
+      <c r="S18" s="24"/>
+      <c r="T18" s="31"/>
       <c r="U18" s="8"/>
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
@@ -5103,10 +5088,10 @@
       <c r="AB18" s="3"/>
       <c r="AC18" s="3"/>
       <c r="AD18" s="3"/>
-      <c r="AE18" s="47"/>
+      <c r="AE18" s="31"/>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
+      <c r="A19" s="38"/>
       <c r="B19" s="5">
         <v>11</v>
       </c>
@@ -5134,34 +5119,34 @@
       <c r="J19" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K19" s="40">
-        <v>4</v>
-      </c>
-      <c r="L19" s="40">
-        <v>2</v>
-      </c>
-      <c r="M19" s="40">
-        <v>2</v>
-      </c>
-      <c r="N19" s="40">
-        <v>1</v>
-      </c>
-      <c r="O19" s="40">
-        <v>1</v>
-      </c>
-      <c r="P19" s="40">
-        <v>4</v>
-      </c>
-      <c r="Q19" s="40">
-        <v>2</v>
-      </c>
-      <c r="R19" s="40">
-        <v>2</v>
-      </c>
-      <c r="S19" s="40">
-        <v>4</v>
-      </c>
-      <c r="T19" s="46">
+      <c r="K19" s="25">
+        <v>4</v>
+      </c>
+      <c r="L19" s="25">
+        <v>2</v>
+      </c>
+      <c r="M19" s="25">
+        <v>2</v>
+      </c>
+      <c r="N19" s="25">
+        <v>1</v>
+      </c>
+      <c r="O19" s="25">
+        <v>1</v>
+      </c>
+      <c r="P19" s="25">
+        <v>4</v>
+      </c>
+      <c r="Q19" s="25">
+        <v>2</v>
+      </c>
+      <c r="R19" s="25">
+        <v>2</v>
+      </c>
+      <c r="S19" s="25">
+        <v>4</v>
+      </c>
+      <c r="T19" s="40">
         <v>0.10694444444444444</v>
       </c>
       <c r="U19" s="8" t="s">
@@ -5194,12 +5179,12 @@
       <c r="AD19" s="9">
         <v>1</v>
       </c>
-      <c r="AE19" s="46">
+      <c r="AE19" s="40">
         <v>2.4999999999999998E-2</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
+      <c r="A20" s="38"/>
       <c r="B20" s="5">
         <v>12</v>
       </c>
@@ -5227,34 +5212,34 @@
       <c r="J20" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K20" s="40">
+      <c r="K20" s="25">
         <v>3</v>
       </c>
-      <c r="L20" s="40">
-        <v>2</v>
-      </c>
-      <c r="M20" s="40">
-        <v>2</v>
-      </c>
-      <c r="N20" s="40">
+      <c r="L20" s="25">
+        <v>2</v>
+      </c>
+      <c r="M20" s="25">
+        <v>2</v>
+      </c>
+      <c r="N20" s="25">
         <v>3</v>
       </c>
-      <c r="O20" s="40">
-        <v>1</v>
-      </c>
-      <c r="P20" s="40">
+      <c r="O20" s="25">
+        <v>1</v>
+      </c>
+      <c r="P20" s="25">
         <v>3</v>
       </c>
-      <c r="Q20" s="40">
-        <v>4</v>
-      </c>
-      <c r="R20" s="40">
-        <v>4</v>
-      </c>
-      <c r="S20" s="40">
-        <v>2</v>
-      </c>
-      <c r="T20" s="46"/>
+      <c r="Q20" s="25">
+        <v>4</v>
+      </c>
+      <c r="R20" s="25">
+        <v>4</v>
+      </c>
+      <c r="S20" s="25">
+        <v>2</v>
+      </c>
+      <c r="T20" s="40"/>
       <c r="U20" s="8" t="s">
         <v>12</v>
       </c>
@@ -5285,97 +5270,97 @@
       <c r="AD20" s="9">
         <v>1</v>
       </c>
-      <c r="AE20" s="46"/>
+      <c r="AE20" s="40"/>
     </row>
-    <row r="21" spans="1:31" s="43" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="43" t="s">
+    <row r="21" spans="1:31" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="45">
+      <c r="C21" s="30">
         <f>AVERAGE(C13:C20)</f>
         <v>23.166666666666668</v>
       </c>
-      <c r="H21" s="45">
+      <c r="H21" s="30">
         <f>AVERAGE(H13:H20)</f>
         <v>4.166666666666667</v>
       </c>
-      <c r="K21" s="44">
+      <c r="K21" s="29">
         <f>AVERAGE(K13:K20)</f>
         <v>3.8333333333333335</v>
       </c>
-      <c r="L21" s="44">
+      <c r="L21" s="29">
         <f t="shared" ref="L21:S21" si="2">AVERAGE(L13:L20)</f>
         <v>3.3333333333333335</v>
       </c>
-      <c r="M21" s="44">
+      <c r="M21" s="29">
         <f t="shared" si="2"/>
         <v>2.6666666666666665</v>
       </c>
-      <c r="N21" s="44">
+      <c r="N21" s="29">
         <f t="shared" si="2"/>
         <v>3.3333333333333335</v>
       </c>
-      <c r="O21" s="44">
+      <c r="O21" s="29">
         <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
-      <c r="P21" s="44">
+      <c r="P21" s="29">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="Q21" s="44">
+      <c r="Q21" s="29">
         <f t="shared" si="2"/>
         <v>3.5</v>
       </c>
-      <c r="R21" s="44">
+      <c r="R21" s="29">
         <f t="shared" si="2"/>
         <v>3.8333333333333335</v>
       </c>
-      <c r="S21" s="44">
+      <c r="S21" s="29">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="T21" s="48">
+      <c r="T21" s="32">
         <f>AVERAGE(T13:T20)</f>
         <v>9.2824074074074073E-2</v>
       </c>
-      <c r="V21" s="43">
+      <c r="V21" s="28">
         <f>AVERAGE(V13:V20)</f>
         <v>4.833333333333333</v>
       </c>
-      <c r="W21" s="43">
+      <c r="W21" s="28">
         <f t="shared" ref="W21:AD21" si="3">AVERAGE(W13:W20)</f>
         <v>4.666666666666667</v>
       </c>
-      <c r="X21" s="43">
+      <c r="X21" s="28">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="Y21" s="43">
+      <c r="Y21" s="28">
         <f t="shared" si="3"/>
         <v>4.833333333333333</v>
       </c>
-      <c r="Z21" s="43">
+      <c r="Z21" s="28">
         <f t="shared" si="3"/>
         <v>3.8333333333333335</v>
       </c>
-      <c r="AA21" s="43">
+      <c r="AA21" s="28">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="AB21" s="43">
+      <c r="AB21" s="28">
         <f t="shared" si="3"/>
         <v>1.3333333333333333</v>
       </c>
-      <c r="AC21" s="43">
+      <c r="AC21" s="28">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="AD21" s="43">
+      <c r="AD21" s="28">
         <f t="shared" si="3"/>
         <v>1.3333333333333333</v>
       </c>
-      <c r="AE21" s="48">
+      <c r="AE21" s="32">
         <f>AVERAGE(AE13:AE20)</f>
         <v>2.2453703703703701E-2</v>
       </c>
@@ -5386,13 +5371,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A13:A20"/>
-    <mergeCell ref="T13:T14"/>
-    <mergeCell ref="AE13:AE14"/>
-    <mergeCell ref="T16:T17"/>
-    <mergeCell ref="AE16:AE17"/>
-    <mergeCell ref="T19:T20"/>
-    <mergeCell ref="AE19:AE20"/>
     <mergeCell ref="C1:I1"/>
     <mergeCell ref="J1:T1"/>
     <mergeCell ref="U1:AE1"/>
@@ -5403,6 +5381,13 @@
     <mergeCell ref="AE7:AE8"/>
     <mergeCell ref="T10:T11"/>
     <mergeCell ref="AE10:AE11"/>
+    <mergeCell ref="A13:A20"/>
+    <mergeCell ref="T13:T14"/>
+    <mergeCell ref="AE13:AE14"/>
+    <mergeCell ref="T16:T17"/>
+    <mergeCell ref="AE16:AE17"/>
+    <mergeCell ref="T19:T20"/>
+    <mergeCell ref="AE19:AE20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -5415,10 +5400,10 @@
   <dimension ref="A1:AE25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="K9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="X20" sqref="X20"/>
+      <selection pane="bottomRight" activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5428,41 +5413,41 @@
   <sheetData>
     <row r="1" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="5"/>
-      <c r="C1" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="11" t="s">
+      <c r="C1" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="11" t="s">
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="51"/>
+      <c r="U1" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="12"/>
-      <c r="AC1" s="12"/>
-      <c r="AD1" s="12"/>
-      <c r="AE1" s="13"/>
+      <c r="V1" s="50"/>
+      <c r="W1" s="50"/>
+      <c r="X1" s="50"/>
+      <c r="Y1" s="50"/>
+      <c r="Z1" s="50"/>
+      <c r="AA1" s="50"/>
+      <c r="AB1" s="50"/>
+      <c r="AC1" s="50"/>
+      <c r="AD1" s="50"/>
+      <c r="AE1" s="51"/>
     </row>
     <row r="2" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -5518,7 +5503,7 @@
       <c r="S2" s="2">
         <v>9</v>
       </c>
-      <c r="T2" s="19" t="s">
+      <c r="T2" s="11" t="s">
         <v>17</v>
       </c>
       <c r="U2" s="2"/>
@@ -5549,12 +5534,12 @@
       <c r="AD2" s="2">
         <v>9</v>
       </c>
-      <c r="AE2" s="19" t="s">
+      <c r="AE2" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="52" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="5">
@@ -5611,7 +5596,7 @@
       <c r="S3" s="3">
         <v>4</v>
       </c>
-      <c r="T3" s="22">
+      <c r="T3" s="47">
         <v>2.7083333333333334E-2</v>
       </c>
       <c r="U3" s="3" t="s">
@@ -5644,12 +5629,12 @@
       <c r="AD3" s="3">
         <v>1</v>
       </c>
-      <c r="AE3" s="22">
+      <c r="AE3" s="47">
         <v>2.7083333333333334E-2</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
+      <c r="A4" s="44"/>
       <c r="B4" s="5">
         <v>2</v>
       </c>
@@ -5704,7 +5689,7 @@
       <c r="S4" s="3">
         <v>1</v>
       </c>
-      <c r="T4" s="20"/>
+      <c r="T4" s="46"/>
       <c r="U4" s="3" t="s">
         <v>12</v>
       </c>
@@ -5735,10 +5720,10 @@
       <c r="AD4" s="3">
         <v>2</v>
       </c>
-      <c r="AE4" s="20"/>
+      <c r="AE4" s="46"/>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
+      <c r="A5" s="44"/>
       <c r="B5" s="5"/>
       <c r="C5" s="8"/>
       <c r="D5" s="3"/>
@@ -5771,7 +5756,7 @@
       <c r="AE5" s="5"/>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="5">
         <v>3</v>
       </c>
@@ -5826,7 +5811,7 @@
       <c r="S6" s="3">
         <v>1</v>
       </c>
-      <c r="T6" s="23">
+      <c r="T6" s="45">
         <v>3.9583333333333331E-2</v>
       </c>
       <c r="U6" s="3" t="s">
@@ -5859,12 +5844,12 @@
       <c r="AD6" s="3">
         <v>1</v>
       </c>
-      <c r="AE6" s="23">
+      <c r="AE6" s="45">
         <v>2.2916666666666669E-2</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="5">
         <v>4</v>
       </c>
@@ -5919,7 +5904,7 @@
       <c r="S7" s="3">
         <v>2</v>
       </c>
-      <c r="T7" s="20"/>
+      <c r="T7" s="46"/>
       <c r="U7" s="9" t="s">
         <v>12</v>
       </c>
@@ -5950,10 +5935,10 @@
       <c r="AD7" s="3">
         <v>1</v>
       </c>
-      <c r="AE7" s="20"/>
+      <c r="AE7" s="46"/>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="5"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -5986,7 +5971,7 @@
       <c r="AE8" s="5"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="5">
         <v>5</v>
       </c>
@@ -6041,7 +6026,7 @@
       <c r="S9" s="9">
         <v>4</v>
       </c>
-      <c r="T9" s="23">
+      <c r="T9" s="45">
         <v>4.3750000000000004E-2</v>
       </c>
       <c r="U9" s="9" t="s">
@@ -6074,12 +6059,12 @@
       <c r="AD9" s="9">
         <v>2</v>
       </c>
-      <c r="AE9" s="23">
+      <c r="AE9" s="45">
         <v>4.7916666666666663E-2</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
+      <c r="A10" s="53"/>
       <c r="B10" s="4">
         <v>6</v>
       </c>
@@ -6134,7 +6119,7 @@
       <c r="S10" s="2">
         <v>4</v>
       </c>
-      <c r="T10" s="21"/>
+      <c r="T10" s="48"/>
       <c r="U10" s="2" t="s">
         <v>9</v>
       </c>
@@ -6165,10 +6150,10 @@
       <c r="AD10" s="2">
         <v>2</v>
       </c>
-      <c r="AE10" s="21"/>
+      <c r="AE10" s="48"/>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="37" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="5">
@@ -6225,7 +6210,7 @@
       <c r="S11" s="9">
         <v>2</v>
       </c>
-      <c r="T11" s="22">
+      <c r="T11" s="47">
         <v>0.1111111111111111</v>
       </c>
       <c r="U11" s="8" t="s">
@@ -6258,12 +6243,12 @@
       <c r="AD11" s="9">
         <v>2</v>
       </c>
-      <c r="AE11" s="22">
+      <c r="AE11" s="47">
         <v>1.8749999999999999E-2</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
+      <c r="A12" s="38"/>
       <c r="B12" s="5">
         <v>8</v>
       </c>
@@ -6318,7 +6303,7 @@
       <c r="S12" s="9">
         <v>2</v>
       </c>
-      <c r="T12" s="20"/>
+      <c r="T12" s="46"/>
       <c r="U12" s="8" t="s">
         <v>12</v>
       </c>
@@ -6349,17 +6334,17 @@
       <c r="AD12" s="9">
         <v>2</v>
       </c>
-      <c r="AE12" s="20"/>
+      <c r="AE12" s="46"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
+      <c r="A13" s="38"/>
       <c r="B13" s="5"/>
       <c r="I13" s="5"/>
       <c r="T13" s="5"/>
       <c r="AE13" s="5"/>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
+      <c r="A14" s="38"/>
       <c r="B14" s="5">
         <v>9</v>
       </c>
@@ -6414,7 +6399,7 @@
       <c r="S14" s="9">
         <v>1</v>
       </c>
-      <c r="T14" s="23">
+      <c r="T14" s="45">
         <v>6.0416666666666667E-2</v>
       </c>
       <c r="U14" s="10" t="s">
@@ -6447,12 +6432,12 @@
       <c r="AD14" s="9">
         <v>1</v>
       </c>
-      <c r="AE14" s="23">
+      <c r="AE14" s="45">
         <v>2.361111111111111E-2</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
+      <c r="A15" s="38"/>
       <c r="B15" s="5">
         <v>10</v>
       </c>
@@ -6507,7 +6492,7 @@
       <c r="S15" s="9">
         <v>1</v>
       </c>
-      <c r="T15" s="20"/>
+      <c r="T15" s="46"/>
       <c r="U15" s="8" t="s">
         <v>12</v>
       </c>
@@ -6538,10 +6523,10 @@
       <c r="AD15" s="9">
         <v>1</v>
       </c>
-      <c r="AE15" s="20"/>
+      <c r="AE15" s="46"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
+      <c r="A16" s="38"/>
       <c r="B16" s="5"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -6574,7 +6559,7 @@
       <c r="AE16" s="5"/>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
+      <c r="A17" s="38"/>
       <c r="B17" s="5">
         <v>11</v>
       </c>
@@ -6629,7 +6614,7 @@
       <c r="S17" s="9">
         <v>4</v>
       </c>
-      <c r="T17" s="23">
+      <c r="T17" s="45">
         <v>0.10694444444444444</v>
       </c>
       <c r="U17" s="8" t="s">
@@ -6662,12 +6647,12 @@
       <c r="AD17" s="9">
         <v>1</v>
       </c>
-      <c r="AE17" s="23">
+      <c r="AE17" s="45">
         <v>2.4999999999999998E-2</v>
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
+      <c r="A18" s="38"/>
       <c r="B18" s="5">
         <v>12</v>
       </c>
@@ -6722,7 +6707,7 @@
       <c r="S18" s="9">
         <v>2</v>
       </c>
-      <c r="T18" s="20"/>
+      <c r="T18" s="46"/>
       <c r="U18" s="8" t="s">
         <v>12</v>
       </c>
@@ -6753,7 +6738,7 @@
       <c r="AD18" s="9">
         <v>1</v>
       </c>
-      <c r="AE18" s="20"/>
+      <c r="AE18" s="46"/>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="K19" s="1"/>
@@ -6762,7 +6747,9 @@
       <c r="U25" s="1"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="17">
+    <mergeCell ref="AE17:AE18"/>
     <mergeCell ref="AE14:AE15"/>
     <mergeCell ref="AE11:AE12"/>
     <mergeCell ref="AE9:AE10"/>
@@ -6779,7 +6766,6 @@
     <mergeCell ref="T3:T4"/>
     <mergeCell ref="AE3:AE4"/>
     <mergeCell ref="AE6:AE7"/>
-    <mergeCell ref="AE17:AE18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>